<commit_message>
[FIX] added missing/recently added boardGame fields to export template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/exports/xlsx/BoardGamesTemplate.xlsx
+++ b/src/main/resources/templates/exports/xlsx/BoardGamesTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Názov Hry</t>
   </si>
   <si>
+    <t xml:space="preserve">Popis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Min. počet hráčov</t>
   </si>
   <si>
@@ -37,6 +40,18 @@
     <t xml:space="preserve">Doba hrania (v min)</t>
   </si>
   <si>
+    <t xml:space="preserve">Vek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kooperatívna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rozšírenie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jednorázová</t>
+  </si>
+  <si>
     <t xml:space="preserve">Autori</t>
   </si>
   <si>
@@ -46,6 +61,9 @@
     <t xml:space="preserve">${title}</t>
   </si>
   <si>
+    <t xml:space="preserve">${description}</t>
+  </si>
+  <si>
     <t xml:space="preserve">${minPlayers}</t>
   </si>
   <si>
@@ -53,6 +71,18 @@
   </si>
   <si>
     <t xml:space="preserve">${playTime}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${ageRange}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${isCooperative}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${isExtension}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${isOneTimePlay}</t>
   </si>
   <si>
     <t xml:space="preserve">${authors}</t>
@@ -238,7 +268,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -246,14 +276,17 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="51.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="51.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,25 +308,55 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CODERVIEW][REFACTOR] updated boardGame export template + hidden description and tutorialUrl from search services
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/exports/xlsx/BoardGamesTemplate.xlsx
+++ b/src/main/resources/templates/exports/xlsx/BoardGamesTemplate.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$C$1:$J$2</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -25,10 +28,7 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Názov Hry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Popis</t>
+    <t xml:space="preserve">Názov</t>
   </si>
   <si>
     <t xml:space="preserve">Min. počet hráčov</t>
@@ -55,15 +55,15 @@
     <t xml:space="preserve">Autori</t>
   </si>
   <si>
+    <t xml:space="preserve">Videonávod</t>
+  </si>
+  <si>
     <t xml:space="preserve">${id}</t>
   </si>
   <si>
     <t xml:space="preserve">${title}</t>
   </si>
   <si>
-    <t xml:space="preserve">${description}</t>
-  </si>
-  <si>
     <t xml:space="preserve">${minPlayers}</t>
   </si>
   <si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">${authors}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${tutorialUrl}</t>
   </si>
 </sst>
 </file>
@@ -263,6 +266,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -276,17 +283,19 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="51.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="51.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,6 +369,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:J2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -367,5 +377,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[FIX] bug reports #4, #5, #6
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/exports/xlsx/BoardGamesTemplate.xlsx
+++ b/src/main/resources/templates/exports/xlsx/BoardGamesTemplate.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$C$1:$J$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$C$1:$K$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">Jednorázová</t>
   </si>
   <si>
+    <t xml:space="preserve">Rok vydania</t>
+  </si>
+  <si>
     <t xml:space="preserve">Autori</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">${isOneTimePlay}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${year}</t>
   </si>
   <si>
     <t xml:space="preserve">${authors}</t>
@@ -275,7 +281,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -283,7 +289,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.46"/>
@@ -293,9 +299,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="51.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="50.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="51.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="50.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,44 +338,50 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:J2"/>
+  <autoFilter ref="C1:K2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>